<commit_message>
Fin code C partie 2 - manque correction VHDL
</commit_message>
<xml_diff>
--- a/Labo5/plan_adresse.xlsx
+++ b/Labo5/plan_adresse.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEIG\S6\SOCF\Laboratoires\Labo5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19000068-0520-4060-BFCA-CDB8E3E1B0CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FBE4B9-2892-4042-8D00-AFC008C7D2BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A896FA24-33D4-42C2-8340-2E03DA34357D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>N</t>
   </si>
@@ -96,12 +96,6 @@
   </si>
   <si>
     <t>[31..4] '0..0' - [3..0] dataKeys (3..0)</t>
-  </si>
-  <si>
-    <t>[31..4] '0..0' - [3..0] interruptmask (3..0)</t>
-  </si>
-  <si>
-    <t>[31..4] reserved - [3..0] interruptmask (3..0)</t>
   </si>
   <si>
     <t>0x0000 0204</t>
@@ -234,6 +228,15 @@
       </rPr>
       <t>0</t>
     </r>
+  </si>
+  <si>
+    <t>[31..4] '0..0' - [3..0] sourceIRQ (3..0)</t>
+  </si>
+  <si>
+    <t>0x0000 0208</t>
+  </si>
+  <si>
+    <t>[31..4] '0..0' - [3..0] maskIRQ (3..0)</t>
   </si>
 </sst>
 </file>
@@ -286,7 +289,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,18 +316,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -417,11 +414,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -471,32 +477,35 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A0EFD5-10C5-44C9-B8AA-F6E05159816F}">
-  <dimension ref="C4:G27"/>
+  <dimension ref="C4:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G28" sqref="C5:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,11 +841,11 @@
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>49</v>
+      <c r="E5" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>12</v>
@@ -855,7 +864,7 @@
       <c r="F6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="24" t="s">
         <v>14</v>
       </c>
     </row>
@@ -872,7 +881,7 @@
       <c r="F7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="7">
@@ -882,12 +891,12 @@
         <v>7</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="25"/>
+        <v>46</v>
+      </c>
+      <c r="G8" s="22"/>
     </row>
     <row r="9" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C9" s="7">
@@ -897,12 +906,12 @@
         <v>8</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="25"/>
+        <v>46</v>
+      </c>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="7">
@@ -912,12 +921,12 @@
         <v>17</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="25"/>
+        <v>46</v>
+      </c>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="7">
@@ -927,27 +936,27 @@
         <v>16</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="25"/>
+        <v>46</v>
+      </c>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="25"/>
+        <v>46</v>
+      </c>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="7">
@@ -962,24 +971,24 @@
       <c r="F13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="25"/>
+        <v>46</v>
+      </c>
+      <c r="G14" s="22"/>
     </row>
     <row r="15" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="7">
@@ -994,7 +1003,7 @@
       <c r="F15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="27" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1003,190 +1012,204 @@
         <v>129</v>
       </c>
       <c r="D16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="27"/>
+    </row>
+    <row r="17" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="7">
+        <v>130</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="27"/>
+    </row>
+    <row r="18" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="22"/>
+    </row>
+    <row r="19" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="7">
+        <v>192</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="22"/>
-    </row>
-    <row r="17" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="15" t="s">
+      <c r="F19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="25"/>
-    </row>
-    <row r="18" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="7">
-        <v>192</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="E20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="22"/>
+    </row>
+    <row r="21" spans="3:7" ht="65.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="7">
+        <v>256</v>
+      </c>
+      <c r="D21" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="23" t="s">
+      <c r="E21" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="7">
-        <v>256</v>
-      </c>
-      <c r="D20" s="13" t="s">
+      <c r="F21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="7">
-        <v>260</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="24"/>
+      <c r="G21" s="21" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="7">
-        <v>264</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>31</v>
+        <v>260</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G22" s="24"/>
+        <v>42</v>
+      </c>
+      <c r="G22" s="21"/>
     </row>
     <row r="23" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C23" s="7">
-        <v>268</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>32</v>
+        <v>264</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>29</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="24"/>
+        <v>41</v>
+      </c>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C24" s="7">
-        <v>272</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>33</v>
+        <v>268</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G24" s="24"/>
+        <v>40</v>
+      </c>
+      <c r="G24" s="21"/>
     </row>
     <row r="25" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C25" s="7">
+        <v>272</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="21"/>
+    </row>
+    <row r="26" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="7">
         <v>276</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" s="24"/>
-    </row>
-    <row r="26" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="21"/>
+    </row>
+    <row r="27" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G26" s="25"/>
-    </row>
-    <row r="27" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C27" s="7">
+      <c r="E27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="22"/>
+    </row>
+    <row r="28" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="7">
         <v>1023</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" s="26"/>
+      <c r="D28" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G20:G25"/>
+    <mergeCell ref="G15:G17"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>